<commit_message>
new scenario file inputs were generated because of creating the edited c_input file. There should be no changes to them, but they need to be commited here because they're new.
</commit_message>
<xml_diff>
--- a/inputs/BaseProtect_HighManage_frst2Xmort_fire.xlsx
+++ b/inputs/BaseProtect_HighManage_frst2Xmort_fire.xlsx
@@ -359,7 +359,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mm/dd/yyyy hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy hh:mm:ss"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -409,7 +409,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="true">
       <alignment wrapText="true"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyNumberFormat="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyNumberFormat="true">
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
@@ -419,7 +419,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>

</xml_diff>